<commit_message>
add frame use time
</commit_message>
<xml_diff>
--- a/_resource/excel/Y-邮件-玩家属性-(框架维护,请勿修改).xlsx
+++ b/_resource/excel/Y-邮件-玩家属性-(框架维护,请勿修改).xlsx
@@ -262,9 +262,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>成就</t>
-  </si>
-  <si>
     <t>uint32</t>
   </si>
   <si>
@@ -407,6 +404,10 @@
   </si>
   <si>
     <t>#mailclass</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -982,7 +983,7 @@
   <dimension ref="A1:AJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1022,7 +1023,7 @@
     <row r="1" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A1" s="8"/>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1098,7 +1099,7 @@
         <v>10</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>11</v>
@@ -1318,10 +1319,10 @@
         <v>38</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>39</v>
@@ -1389,19 +1390,19 @@
     </row>
     <row r="5" spans="1:36" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>56</v>
@@ -1463,13 +1464,13 @@
         <v>56</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P6" s="11">
         <v>0</v>
@@ -1522,16 +1523,16 @@
     </row>
     <row r="7" spans="1:36" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P7" s="11">
         <v>0</v>
@@ -1584,16 +1585,16 @@
     </row>
     <row r="8" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="P8" s="11">
         <v>0</v>
@@ -1646,16 +1647,16 @@
     </row>
     <row r="9" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P9" s="11">
         <v>0</v>
@@ -1708,16 +1709,16 @@
     </row>
     <row r="10" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="E10" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P10" s="11">
         <v>0</v>
@@ -1770,16 +1771,16 @@
     </row>
     <row r="11" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="P11" s="11">
         <v>0</v>
@@ -1832,16 +1833,16 @@
     </row>
     <row r="12" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P12" s="11">
         <v>0</v>
@@ -1894,16 +1895,16 @@
     </row>
     <row r="13" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="P13" s="11">
         <v>0</v>
@@ -1956,16 +1957,16 @@
     </row>
     <row r="14" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="P14" s="11">
         <v>0</v>
@@ -2018,16 +2019,16 @@
     </row>
     <row r="15" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="P15" s="11">
         <v>0</v>
@@ -2080,16 +2081,16 @@
     </row>
     <row r="16" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="E16" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P16" s="11">
         <v>0</v>
@@ -2142,16 +2143,16 @@
     </row>
     <row r="17" spans="1:31" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="P17" s="11">
         <v>0</v>
@@ -2204,16 +2205,16 @@
     </row>
     <row r="18" spans="1:31" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="P18" s="11">
         <v>0</v>

</xml_diff>